<commit_message>
Version 2 PCB_CPU y Version 3 BOM_CPU
Cambios menores en el lettering del PCB.

Cambios en la BOM para adecuarse a la  version 2 de la CPU.
</commit_message>
<xml_diff>
--- a/02.HARDWARE/V2-ROVER-1K/02.BOM/BATT_CPU.xlsx
+++ b/02.HARDWARE/V2-ROVER-1K/02.BOM/BATT_CPU.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/reozen/Team Dropbox/David Garrido/MUSOTOKU/PROJECTS/BATTERYPACK - FALCON/00.REPOSITORIES/BATTERY-PACK/02.HARDWARE/V2-ROVER-1K/02.BOM/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Javi\TEAMDR~1\JRODRI~1\Repositorios\01.Rover\02.HARDWARE\V2-ROVER-1K\02.BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB557A2A-DF8F-1E40-9EC9-AB5CECC4F055}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E4F803D-6F6C-434C-9B1F-7F139D55F03E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19180" yWindow="500" windowWidth="19120" windowHeight="19680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BATT_CPU" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="103">
   <si>
     <t>Qty</t>
   </si>
@@ -192,9 +192,6 @@
     <t>R4, R14, R16, R18</t>
   </si>
   <si>
-    <t>C3, C5, C7, C9, C10, C11, C13, C15, C16, C17, C18, C19, C24, C25, C26, C27</t>
-  </si>
-  <si>
     <t>R48</t>
   </si>
   <si>
@@ -328,6 +325,12 @@
   </si>
   <si>
     <t xml:space="preserve"> +34 603486681</t>
+  </si>
+  <si>
+    <t>C3, C5, C7, C9, C10, C11, C13, C15, C16, C17, C18, C19, C24, C25, C26, C27,C28</t>
+  </si>
+  <si>
+    <t>Se añade en la posicion 12 el part C28 aumentando la cantidad a 17</t>
   </si>
 </sst>
 </file>
@@ -1000,7 +1003,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1013,14 +1016,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="35" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1030,23 +1032,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="42"/>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="24" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1062,51 +1051,63 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Bueno" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Cálculo" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Celda de comprobación" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Celda vinculada" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Encabezado 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Encabezado 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Énfasis1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Énfasis2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Énfasis3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Énfasis4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Énfasis5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Énfasis6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Entrada" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Hipervínculo" xfId="42" builtinId="8"/>
+    <cellStyle name="Incorrecto" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Notas" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Salida" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Texto de advertencia" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Texto explicativo" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Título" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Título 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="6">
     <dxf>
@@ -1219,7 +1220,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1515,120 +1516,120 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N34"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="122.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="122.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" ht="26" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="27" x14ac:dyDescent="0.4">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="D3" s="5"/>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:14" ht="26" x14ac:dyDescent="0.25">
-      <c r="C4" s="15" t="s">
+    <row r="4" spans="1:8" ht="27" x14ac:dyDescent="0.4">
+      <c r="C4" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="17"/>
-    </row>
-    <row r="5" spans="1:14" s="6" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="7"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="9"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="10" t="s">
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="23"/>
+    </row>
+    <row r="5" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C5" s="6"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="8"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="C6" s="10" t="s">
+      <c r="B6" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C6" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="F6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G6" s="10" t="s">
+      <c r="G6" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="10" t="s">
+      <c r="H6" s="9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C7" s="1">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E7" t="s">
         <v>41</v>
       </c>
       <c r="F7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G7" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C8" s="1">
         <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E8" t="s">
         <v>30</v>
@@ -1640,12 +1641,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C9" s="1">
         <v>2</v>
@@ -1662,21 +1663,19 @@
       <c r="G9" t="s">
         <v>17</v>
       </c>
-      <c r="M9" s="13"/>
-      <c r="N9" s="13"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C10" s="1">
         <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E10" t="s">
         <v>31</v>
@@ -1687,21 +1686,19 @@
       <c r="G10" t="s">
         <v>18</v>
       </c>
-      <c r="M10" s="13"/>
-      <c r="N10" s="13"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C11" s="1">
         <v>2</v>
       </c>
       <c r="D11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E11" t="s">
         <v>33</v>
@@ -1712,21 +1709,19 @@
       <c r="G11" t="s">
         <v>18</v>
       </c>
-      <c r="M11" s="13"/>
-      <c r="N11" s="13"/>
-    </row>
-    <row r="12" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C12" s="1">
-        <v>16</v>
-      </c>
-      <c r="D12" s="12" t="s">
-        <v>56</v>
+        <v>17</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>101</v>
       </c>
       <c r="E12" t="s">
         <v>26</v>
@@ -1737,46 +1732,42 @@
       <c r="G12" t="s">
         <v>17</v>
       </c>
-      <c r="M12" s="13"/>
-      <c r="N12" s="13"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C13" s="1">
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E13" t="s">
         <v>40</v>
       </c>
       <c r="F13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G13" t="s">
         <v>19</v>
       </c>
-      <c r="M13" s="13"/>
-      <c r="N13" s="13"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C14" s="1">
         <v>3</v>
       </c>
       <c r="D14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E14" t="s">
         <v>38</v>
@@ -1787,24 +1778,22 @@
       <c r="G14" t="s">
         <v>47</v>
       </c>
-      <c r="H14" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="M14" s="13"/>
-      <c r="N14" s="13"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="H14" s="12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C15" s="1">
         <v>2</v>
       </c>
       <c r="D15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E15" t="s">
         <v>5</v>
@@ -1815,21 +1804,19 @@
       <c r="G15" t="s">
         <v>6</v>
       </c>
-      <c r="M15" s="13"/>
-      <c r="N15" s="13"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C16" s="1">
         <v>3</v>
       </c>
       <c r="D16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E16" t="s">
         <v>35</v>
@@ -1840,15 +1827,13 @@
       <c r="G16" t="s">
         <v>17</v>
       </c>
-      <c r="M16" s="13"/>
-      <c r="N16" s="13"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>11</v>
       </c>
       <c r="B17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C17" s="1">
         <v>1</v>
@@ -1865,15 +1850,13 @@
       <c r="G17" t="s">
         <v>17</v>
       </c>
-      <c r="M17" s="13"/>
-      <c r="N17" s="13"/>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C18" s="1">
         <v>1</v>
@@ -1890,21 +1873,19 @@
       <c r="G18" t="s">
         <v>17</v>
       </c>
-      <c r="M18" s="13"/>
-      <c r="N18" s="13"/>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>13</v>
       </c>
       <c r="B19" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C19" s="1">
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E19" t="s">
         <v>29</v>
@@ -1915,21 +1896,19 @@
       <c r="G19" t="s">
         <v>17</v>
       </c>
-      <c r="M19" s="13"/>
-      <c r="N19" s="13"/>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C20" s="1">
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E20" t="s">
         <v>36</v>
@@ -1940,15 +1919,13 @@
       <c r="G20" t="s">
         <v>17</v>
       </c>
-      <c r="M20" s="13"/>
-      <c r="N20" s="13"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>15</v>
       </c>
       <c r="B21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C21" s="1">
         <v>4</v>
@@ -1965,21 +1942,19 @@
       <c r="G21" t="s">
         <v>17</v>
       </c>
-      <c r="M21" s="13"/>
-      <c r="N21" s="13"/>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>16</v>
       </c>
       <c r="B22" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C22" s="1">
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E22" t="s">
         <v>27</v>
@@ -1990,15 +1965,13 @@
       <c r="G22" t="s">
         <v>17</v>
       </c>
-      <c r="M22" s="13"/>
-      <c r="N22" s="13"/>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>17</v>
       </c>
       <c r="B23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C23" s="1">
         <v>1</v>
@@ -2015,21 +1988,19 @@
       <c r="G23" t="s">
         <v>17</v>
       </c>
-      <c r="M23" s="13"/>
-      <c r="N23" s="13"/>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>18</v>
       </c>
       <c r="B24" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C24" s="1">
         <v>3</v>
       </c>
       <c r="D24" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E24" t="s">
         <v>32</v>
@@ -2040,15 +2011,13 @@
       <c r="G24" t="s">
         <v>17</v>
       </c>
-      <c r="M24" s="13"/>
-      <c r="N24" s="13"/>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>19</v>
       </c>
       <c r="B25" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C25" s="1">
         <v>3</v>
@@ -2065,49 +2034,45 @@
       <c r="G25" t="s">
         <v>17</v>
       </c>
-      <c r="M25" s="13"/>
-      <c r="N25" s="13"/>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>20</v>
       </c>
       <c r="B26" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C26" s="1">
         <v>3</v>
       </c>
       <c r="D26" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E26" t="s">
         <v>42</v>
       </c>
       <c r="F26" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G26" t="s">
         <v>50</v>
       </c>
-      <c r="H26" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="M26" s="13"/>
-      <c r="N26" s="13"/>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="H26" s="12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>21</v>
       </c>
       <c r="B27" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C27" s="1">
         <v>1</v>
       </c>
       <c r="D27" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E27" t="s">
         <v>37</v>
@@ -2118,15 +2083,13 @@
       <c r="G27" t="s">
         <v>46</v>
       </c>
-      <c r="M27" s="13"/>
-      <c r="N27" s="13"/>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>22</v>
       </c>
       <c r="B28" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C28" s="1">
         <v>1</v>
@@ -2143,21 +2106,19 @@
       <c r="G28" t="s">
         <v>52</v>
       </c>
-      <c r="M28" s="13"/>
-      <c r="N28" s="13"/>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>23</v>
       </c>
       <c r="B29" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C29" s="1">
         <v>1</v>
       </c>
       <c r="D29" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E29" t="s">
         <v>39</v>
@@ -2168,21 +2129,19 @@
       <c r="G29" t="s">
         <v>48</v>
       </c>
-      <c r="M29" s="13"/>
-      <c r="N29" s="13"/>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>24</v>
       </c>
       <c r="B30" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C30" s="1">
         <v>1</v>
       </c>
       <c r="D30" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E30" t="s">
         <v>43</v>
@@ -2193,45 +2152,29 @@
       <c r="G30" t="s">
         <v>51</v>
       </c>
-      <c r="M30" s="13"/>
-      <c r="N30" s="13"/>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>25</v>
       </c>
       <c r="B31" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C31" s="1">
         <v>1</v>
       </c>
       <c r="D31" t="s">
-        <v>63</v>
-      </c>
-      <c r="E31" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="E31" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="F31" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="F31" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="G31" s="11" t="s">
+      <c r="G31" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="M31" s="13"/>
-      <c r="N31" s="13"/>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="M32" s="13"/>
-      <c r="N32" s="13"/>
-    </row>
-    <row r="33" spans="13:14" x14ac:dyDescent="0.2">
-      <c r="M33" s="13"/>
-      <c r="N33" s="13"/>
-    </row>
-    <row r="34" spans="13:14" x14ac:dyDescent="0.2">
-      <c r="M34" s="13"/>
-      <c r="N34" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2262,62 +2205,76 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15976B5A-CF8E-C940-9265-A2311480139B}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="46.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="13" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="14" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="19" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
+      <c r="B3" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="C3" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="D3" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="D3" s="19" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
-      <c r="B4" s="20">
+      <c r="B4" s="15">
         <v>44874</v>
       </c>
       <c r="C4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D4" t="s">
         <v>89</v>
       </c>
-      <c r="D4" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
-      <c r="B5" s="20">
+      <c r="B5" s="15">
         <v>44880</v>
       </c>
       <c r="C5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D5" t="s">
         <v>91</v>
       </c>
-      <c r="D5" t="s">
-        <v>92</v>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" s="15">
+        <v>44918</v>
+      </c>
+      <c r="C6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D6" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -2333,72 +2290,72 @@
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.2">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+    </row>
+    <row r="2" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-    </row>
-    <row r="2" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A2" s="22" t="s">
+      <c r="B2" s="16"/>
+      <c r="C2" s="17"/>
+    </row>
+    <row r="3" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="23"/>
-    </row>
-    <row r="3" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A3" s="22" t="s">
+      <c r="B3" s="16"/>
+      <c r="C3" s="17"/>
+    </row>
+    <row r="4" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="16">
+        <v>28805</v>
+      </c>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+    </row>
+    <row r="5" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="23"/>
-    </row>
-    <row r="4" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A4" s="22">
-        <v>28805</v>
-      </c>
-      <c r="B4" s="23"/>
-      <c r="C4" s="23"/>
-    </row>
-    <row r="5" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A5" s="22" t="s">
+      <c r="B5" s="16"/>
+      <c r="C5" s="17"/>
+    </row>
+    <row r="6" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="B5" s="22"/>
-      <c r="C5" s="23"/>
-    </row>
-    <row r="6" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A6" s="22" t="s">
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+    </row>
+    <row r="7" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="16"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+    </row>
+    <row r="8" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
-    </row>
-    <row r="7" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A7" s="22"/>
-      <c r="B7" s="23"/>
-      <c r="C7" s="23"/>
-    </row>
-    <row r="8" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A8" s="24" t="s">
+      <c r="B8" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="B8" s="25" t="s">
+      <c r="C8" s="20"/>
+    </row>
+    <row r="9" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="C8" s="26"/>
-    </row>
-    <row r="9" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A9" s="24" t="s">
+      <c r="B9" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="B9" s="23" t="s">
-        <v>101</v>
-      </c>
-      <c r="C9" s="23"/>
+      <c r="C9" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>